<commit_message>
Search function now works and updated excel
</commit_message>
<xml_diff>
--- a/ProjectFiles/PlanGroup2.xlsx
+++ b/ProjectFiles/PlanGroup2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LudwigOelker\Desktop\Group2FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LudwigOelker\Desktop\Group2\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEB43C5-099A-482F-9042-35C0BBE2ECB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A401E-9778-4900-9576-278D11157F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Day 1</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Search in dummy DB</t>
+  </si>
+  <si>
+    <t>Integrate DB</t>
   </si>
 </sst>
 </file>
@@ -198,19 +201,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +496,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +506,7 @@
     <col min="5" max="5" width="2.77734375" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.77734375" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.77734375" customWidth="1"/>
@@ -523,34 +525,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="F1" s="9">
+      <c r="F1" s="7">
         <v>44949</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="7">
         <v>44950</v>
       </c>
-      <c r="J1" s="9">
+      <c r="J1" s="7">
         <v>44951</v>
       </c>
-      <c r="L1" s="9">
+      <c r="L1" s="7">
         <v>44952</v>
       </c>
-      <c r="N1" s="9">
+      <c r="N1" s="7">
         <v>44953</v>
       </c>
-      <c r="P1" s="9">
+      <c r="P1" s="7">
         <v>44956</v>
       </c>
-      <c r="R1" s="9">
+      <c r="R1" s="7">
         <v>44957</v>
       </c>
-      <c r="T1" s="9">
+      <c r="T1" s="7">
         <v>44958</v>
       </c>
-      <c r="V1" s="9">
+      <c r="V1" s="7">
         <v>44959</v>
       </c>
-      <c r="X1" s="9">
+      <c r="X1" s="7">
         <v>44960</v>
       </c>
     </row>
@@ -559,44 +561,44 @@
         <v>23</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="3" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="3" t="s">
+      <c r="U2" s="3"/>
+      <c r="V2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="3" t="s">
+      <c r="W2" s="3"/>
+      <c r="X2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -607,40 +609,31 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="L3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2" t="s">
+      <c r="P3" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2" t="s">
+      <c r="R3" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2" t="s">
+      <c r="T3" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2" t="s">
+      <c r="V3" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2" t="s">
+      <c r="X3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -651,64 +644,43 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="G4" s="5"/>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
+      <c r="G5" s="5"/>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -716,7 +688,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -731,7 +703,7 @@
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="F10" t="s">
         <v>19</v>
       </c>
@@ -739,7 +711,7 @@
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
       <c r="F11" t="s">
         <v>20</v>
       </c>
@@ -761,13 +733,13 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E14" s="6"/>
+      <c r="E14" s="1"/>
       <c r="F14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E15" s="6"/>
+      <c r="E15" s="5"/>
       <c r="F15" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Renamed HomePage.html, reworked structure
</commit_message>
<xml_diff>
--- a/ProjectFiles/PlanGroup2.xlsx
+++ b/ProjectFiles/PlanGroup2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\JavaProjects\Emotus\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D2A060-E909-4246-AA7A-BB05383FFDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC382E-D751-4120-9055-A75794A49CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Day 1</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Integrate DB</t>
   </si>
   <si>
-    <t>Search opt</t>
-  </si>
-  <si>
     <t>- Search into DB</t>
   </si>
   <si>
@@ -140,10 +137,16 @@
     <t>Day 7 (Sprint 2 end)</t>
   </si>
   <si>
-    <t>Every day start with a stand up and bring up the previous day and discuss what happaened and included incomplete tasks. Stand up at the end to sum what we have done.</t>
-  </si>
-  <si>
     <t>Plan design</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
+  </si>
+  <si>
+    <t>Every day start with a stand up and bring up the previous day and discuss transpired and included incomplete tasks. Stand up at the end to sum what we have done.</t>
+  </si>
+  <si>
+    <t>Search optimization</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,7 +596,7 @@
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="10"/>
       <c r="E2" s="3"/>
@@ -610,7 +613,7 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="2" t="s">
@@ -622,7 +625,7 @@
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="2" t="s">
@@ -630,7 +633,7 @@
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="2" t="s">
@@ -645,28 +648,28 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X3" t="s">
         <v>10</v>
@@ -685,15 +688,19 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -709,11 +716,11 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -729,11 +736,11 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
@@ -749,7 +756,7 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -761,7 +768,7 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -773,7 +780,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -785,7 +792,7 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -797,7 +804,7 @@
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -809,7 +816,7 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated old code and added functionality on Index
</commit_message>
<xml_diff>
--- a/ProjectFiles/PlanGroup2.xlsx
+++ b/ProjectFiles/PlanGroup2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\JavaProjects\Emotus\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520AC083-2A70-441E-B4D2-2A5BDE2530F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C0953-3E07-4773-B36D-3DBCAEA70E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Day 1</t>
   </si>
@@ -281,6 +281,18 @@
   </si>
   <si>
     <t>Loading icon</t>
+  </si>
+  <si>
+    <t>Picture rep</t>
+  </si>
+  <si>
+    <t>Make ppt</t>
+  </si>
+  <si>
+    <t>Logo?</t>
+  </si>
+  <si>
+    <t>Big merge</t>
   </si>
 </sst>
 </file>
@@ -392,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -414,7 +426,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,7 +709,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +729,7 @@
     <col min="15" max="15" width="2.77734375" customWidth="1"/>
     <col min="16" max="16" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="2.77734375" customWidth="1"/>
-    <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.77734375" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="2.77734375" customWidth="1"/>
@@ -871,7 +882,7 @@
         <v>52</v>
       </c>
       <c r="S4" s="5"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -898,9 +909,13 @@
       <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="5"/>
+      <c r="O5" s="1"/>
       <c r="P5" t="s">
         <v>36</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -930,6 +945,10 @@
       <c r="P6" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
@@ -954,6 +973,10 @@
       <c r="P7" t="s">
         <v>77</v>
       </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
@@ -970,6 +993,10 @@
       <c r="P8" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
@@ -982,9 +1009,13 @@
       <c r="H9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="5"/>
+      <c r="O9" s="1"/>
       <c r="P9" t="s">
         <v>78</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -999,8 +1030,12 @@
         <v>22</v>
       </c>
       <c r="O10" s="5"/>
-      <c r="P10" s="15" t="s">
+      <c r="P10" t="s">
         <v>80</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -1013,6 +1048,10 @@
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New API Key and Updated ppt & excel
</commit_message>
<xml_diff>
--- a/ProjectFiles/PlanGroup2.xlsx
+++ b/ProjectFiles/PlanGroup2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Module14\Emotus\ProjectFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\JavaProjects\Emotus\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF05820-FC7C-4A6F-A23C-7D03B146D792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CC7AA-8BB9-4FC8-9230-F4A574DE7D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -763,35 +763,35 @@
   <dimension ref="B1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" customWidth="1"/>
-    <col min="4" max="4" width="3.6328125" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.81640625" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.81640625" customWidth="1"/>
-    <col min="12" max="12" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.81640625" customWidth="1"/>
-    <col min="14" max="14" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.81640625" customWidth="1"/>
-    <col min="16" max="16" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.81640625" customWidth="1"/>
-    <col min="18" max="18" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="5" width="2.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.77734375" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.77734375" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.77734375" customWidth="1"/>
+    <col min="16" max="16" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.77734375" customWidth="1"/>
+    <col min="18" max="18" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.77734375" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.81640625" customWidth="1"/>
+    <col min="21" max="21" width="2.77734375" customWidth="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.81640625" customWidth="1"/>
+    <col min="23" max="23" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F1" s="7">
         <v>44949</v>
       </c>
@@ -823,7 +823,7 @@
         <v>44960</v>
       </c>
     </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>35</v>
       </c>
@@ -869,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="E3" s="1"/>
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="E4" s="1"/>
@@ -935,7 +935,7 @@
       <c r="R4" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="1" t="s">
         <v>99</v>
       </c>
       <c r="T4" t="s">
@@ -946,7 +946,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="E5" s="1"/>
@@ -984,7 +984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="E6" s="1"/>
@@ -1020,7 +1020,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="E7" s="1"/>
@@ -1054,7 +1054,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="E8" s="1"/>
@@ -1080,7 +1080,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="E9" s="1"/>
@@ -1106,7 +1106,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="E10" s="5"/>
@@ -1130,7 +1130,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="E11" s="5"/>
@@ -1152,7 +1152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="E12" s="1"/>
@@ -1170,7 +1170,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="E13" s="1"/>
@@ -1184,7 +1184,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E14" s="1"/>
       <c r="F14" t="s">
         <v>19</v>
@@ -1196,7 +1196,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="E15" s="5"/>
       <c r="F15" t="s">
         <v>20</v>
@@ -1208,7 +1208,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
       <c r="S16" s="5" t="s">
         <v>96</v>
       </c>
@@ -1234,15 +1234,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="2.90625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.90625" customWidth="1"/>
-    <col min="6" max="6" width="2.90625" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="10" t="s">
         <v>37</v>
@@ -1256,7 +1256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>40</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>41</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>40</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>41</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>40</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>41</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>40</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>41</v>
       </c>
@@ -1358,12 +1358,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>67</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>71</v>
       </c>
@@ -1420,32 +1420,32 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Added logo & favicon
</commit_message>
<xml_diff>
--- a/ProjectFiles/PlanGroup2.xlsx
+++ b/ProjectFiles/PlanGroup2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\JavaProjects\Emotus\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CC7AA-8BB9-4FC8-9230-F4A574DE7D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0EF396-A159-4AC3-AE3A-B4E09455A31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Day 1</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Logo</t>
   </si>
   <si>
-    <t>deverse items</t>
-  </si>
-  <si>
     <t>replace dummy texts</t>
   </si>
   <si>
@@ -347,6 +344,15 @@
   </si>
   <si>
     <t>synka bakgrundsfärg</t>
+  </si>
+  <si>
+    <t>Diff search result</t>
+  </si>
+  <si>
+    <t>Navbar ska inte täcka content på någon sida</t>
+  </si>
+  <si>
+    <t>Create unit test for class</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:X16"/>
+  <dimension ref="B1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,7 +791,7 @@
     <col min="17" max="17" width="2.77734375" customWidth="1"/>
     <col min="18" max="18" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.77734375" customWidth="1"/>
-    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="2.77734375" customWidth="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="2.77734375" customWidth="1"/>
@@ -936,7 +942,7 @@
         <v>52</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T4" t="s">
         <v>79</v>
@@ -978,10 +984,14 @@
         <v>76</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T5" t="s">
         <v>85</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -1047,8 +1057,8 @@
       <c r="R7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>100</v>
+      <c r="S7" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="T7" t="s">
         <v>87</v>
@@ -1073,11 +1083,11 @@
       <c r="R8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="S8" s="5" t="s">
-        <v>98</v>
+      <c r="S8" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="T8" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -1099,11 +1109,11 @@
       <c r="R9" t="s">
         <v>81</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>101</v>
+      <c r="S9" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="T9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -1125,9 +1135,9 @@
       <c r="R10" t="s">
         <v>83</v>
       </c>
-      <c r="S10" s="5"/>
+      <c r="S10" s="1"/>
       <c r="T10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -1146,10 +1156,10 @@
         <v>84</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -1163,11 +1173,11 @@
       <c r="H12" t="s">
         <v>23</v>
       </c>
-      <c r="S12" s="5" t="s">
-        <v>97</v>
+      <c r="S12" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="T12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -1177,11 +1187,11 @@
       <c r="F13" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="5" t="s">
-        <v>97</v>
+      <c r="S13" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="T13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -1189,11 +1199,11 @@
       <c r="F14" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="5" t="s">
-        <v>96</v>
+      <c r="S14" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="T14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
@@ -1202,18 +1212,24 @@
         <v>20</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="S16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="S16" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="T16" t="s">
-        <v>95</v>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S17" s="5"/>
+      <c r="T17" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>